<commit_message>
changes done In Admin Create Page Test
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/New_Poject_Details.xlsx
+++ b/TestData/Excel_Files/New_Poject_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92D70EC-9D17-4C07-B149-7A85DEE3258A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424D325E-5A4E-413B-8E5D-63427CF57116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{70774B03-B351-4631-9DE8-6B86FF3E4275}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mmm/yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -152,7 +152,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,13 +579,13 @@
         <v>18</v>
       </c>
       <c r="L2" s="2">
-        <v>35819</v>
+        <v>37201</v>
       </c>
       <c r="M2" s="2">
-        <v>45315</v>
+        <v>48357</v>
       </c>
       <c r="N2" s="2">
-        <v>46046</v>
+        <v>48226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some test case
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/New_Poject_Details.xlsx
+++ b/TestData/Excel_Files/New_Poject_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B2EE67-12B4-4C90-9329-C90E6C874440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332A6EB4-3C6E-4285-AA94-4258F1FA1DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{70774B03-B351-4631-9DE8-6B86FF3E4275}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Project Name</t>
   </si>
   <si>
-    <t>Client Image Path</t>
-  </si>
-  <si>
     <t>Consultant Name</t>
   </si>
   <si>
@@ -156,6 +153,30 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>File Path</t>
+  </si>
+  <si>
+    <t>\\TestData\\Excel_Files\\New_Poject_Details.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Image Path </t>
+  </si>
+  <si>
+    <t>APMS-T12</t>
+  </si>
+  <si>
+    <t>APMS-T27</t>
+  </si>
+  <si>
+    <t>\\src\\test\\resources\\Configuration\\AppData\\Config.properties</t>
+  </si>
+  <si>
+    <t>APMS-T11</t>
+  </si>
+  <si>
+    <t>APMS-T26</t>
   </si>
 </sst>
 </file>
@@ -542,24 +563,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D5353A-A70B-4FBF-B8E0-5139DE62F6E4}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="33.36328125" customWidth="1"/>
-    <col min="7" max="7" width="111.7265625" customWidth="1"/>
+    <col min="5" max="5" width="35.453125" customWidth="1"/>
+    <col min="6" max="6" width="33.36328125" customWidth="1"/>
+    <col min="8" max="8" width="111.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -568,162 +590,199 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="M2" s="1"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3">
+        <v>12345678</v>
+      </c>
+      <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3">
+        <v>1234567890</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="2">
+        <v>45418</v>
+      </c>
+      <c r="O3" s="2">
+        <v>45435</v>
+      </c>
+      <c r="P3" s="2">
+        <v>45670</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="H3">
-        <v>12345678</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3">
-        <v>1234567890</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="2">
-        <v>45418</v>
-      </c>
-      <c r="N3" s="2">
-        <v>45435</v>
-      </c>
-      <c r="O3" s="2">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="M8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="M9" t="s">
         <v>36</v>
       </c>
-      <c r="L9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D11" t="s">
-        <v>22</v>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1" xr:uid="{420182E3-E264-48AD-9427-74F394420E85}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{D7A11380-66F9-4EB0-A962-6BBC0383AD52}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{BB4F4B60-A955-431D-9A6F-D674A0235F5F}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{A5E02953-A716-4FB1-9F94-CBF7B8EB86FB}"/>
-    <hyperlink ref="L8" r:id="rId5" xr:uid="{E466AA4E-62F4-4A07-9470-12321033BF1D}"/>
+    <hyperlink ref="K3" r:id="rId1" xr:uid="{420182E3-E264-48AD-9427-74F394420E85}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{D7A11380-66F9-4EB0-A962-6BBC0383AD52}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{BB4F4B60-A955-431D-9A6F-D674A0235F5F}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{A5E02953-A716-4FB1-9F94-CBF7B8EB86FB}"/>
+    <hyperlink ref="M8" r:id="rId5" xr:uid="{E466AA4E-62F4-4A07-9470-12321033BF1D}"/>
+    <hyperlink ref="E13" r:id="rId6" xr:uid="{EE9855ED-A36D-4831-BB93-633FEAE35580}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed Create Project Test Case
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/New_Poject_Details.xlsx
+++ b/TestData/Excel_Files/New_Poject_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332A6EB4-3C6E-4285-AA94-4258F1FA1DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB563FF-387A-4B53-9F1B-240481A893E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{70774B03-B351-4631-9DE8-6B86FF3E4275}"/>
   </bookViews>
@@ -565,14 +565,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D5353A-A70B-4FBF-B8E0-5139DE62F6E4}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="35.453125" customWidth="1"/>
-    <col min="6" max="6" width="33.36328125" customWidth="1"/>
+    <col min="5" max="5" width="49.1796875" customWidth="1"/>
+    <col min="6" max="6" width="71.54296875" customWidth="1"/>
     <col min="8" max="8" width="111.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -742,7 +742,7 @@
         <v>45</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -750,11 +750,11 @@
       <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -783,6 +783,9 @@
     <hyperlink ref="H3" r:id="rId4" xr:uid="{A5E02953-A716-4FB1-9F94-CBF7B8EB86FB}"/>
     <hyperlink ref="M8" r:id="rId5" xr:uid="{E466AA4E-62F4-4A07-9470-12321033BF1D}"/>
     <hyperlink ref="E13" r:id="rId6" xr:uid="{EE9855ED-A36D-4831-BB93-633FEAE35580}"/>
+    <hyperlink ref="E11" r:id="rId7" xr:uid="{118E441C-31E2-4E4A-BAA0-CED89A1941F6}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{D703EAD6-6487-4B77-90FB-D9AEFE4C648D}"/>
+    <hyperlink ref="H11" r:id="rId9" xr:uid="{9728ACAC-6626-45D1-87FE-2B37E8A86378}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Edited and Add Create Project Details Test Case
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/New_Poject_Details.xlsx
+++ b/TestData/Excel_Files/New_Poject_Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB563FF-387A-4B53-9F1B-240481A893E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CB7CBC-4E07-443D-B574-66658A990774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{70774B03-B351-4631-9DE8-6B86FF3E4275}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>prashant</t>
   </si>
   <si>
-    <t>prashant@123</t>
-  </si>
-  <si>
     <t>abcd@gmail.com</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>APMS-T26</t>
+  </si>
+  <si>
+    <t>Prashant$123</t>
   </si>
 </sst>
 </file>
@@ -565,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D5353A-A70B-4FBF-B8E0-5139DE62F6E4}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -590,10 +590,10 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -608,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L1" t="s">
         <v>7</v>
@@ -623,15 +623,15 @@
         <v>10</v>
       </c>
       <c r="P1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2" s="1"/>
       <c r="M2" s="1"/>
@@ -641,10 +641,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -653,13 +653,13 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3">
         <v>12345678</v>
@@ -668,13 +668,13 @@
         <v>14</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="L3">
         <v>1234567890</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N3" s="2">
         <v>45418</v>
@@ -688,96 +688,96 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" t="s">
         <v>35</v>
-      </c>
-      <c r="M9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" xr:uid="{420182E3-E264-48AD-9427-74F394420E85}"/>
+    <hyperlink ref="K3" r:id="rId1" display="prashant@" xr:uid="{420182E3-E264-48AD-9427-74F394420E85}"/>
     <hyperlink ref="M3" r:id="rId2" xr:uid="{D7A11380-66F9-4EB0-A962-6BBC0383AD52}"/>
     <hyperlink ref="F3" r:id="rId3" xr:uid="{BB4F4B60-A955-431D-9A6F-D674A0235F5F}"/>
     <hyperlink ref="H3" r:id="rId4" xr:uid="{A5E02953-A716-4FB1-9F94-CBF7B8EB86FB}"/>

</xml_diff>

<commit_message>
updated The TestCases of AdminMenuPermissionTest class and Fixed AwtUtills classes and created OmsAdminDashboardPage class
</commit_message>
<xml_diff>
--- a/TestData/Excel_Files/New_Poject_Details.xlsx
+++ b/TestData/Excel_Files/New_Poject_Details.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWT Tester\eclipse-workspace\Awt_Project_Managment\TestData\Excel_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CB7CBC-4E07-443D-B574-66658A990774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAEEE31-0127-40A4-B5D1-2FCEC5D8628E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{70774B03-B351-4631-9DE8-6B86FF3E4275}"/>
   </bookViews>
   <sheets>
     <sheet name="Project_Details" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Project_Details!$F$1:$F$13</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,23 +39,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>TestCaseId</t>
   </si>
   <si>
-    <t>Client Name</t>
-  </si>
-  <si>
     <t>Project Name</t>
   </si>
   <si>
     <t>Consultant Name</t>
   </si>
   <si>
-    <t>Consultant Image Path</t>
-  </si>
-  <si>
     <t>Licenses Key</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Expected Date</t>
   </si>
   <si>
-    <t>Indus Valley</t>
-  </si>
-  <si>
     <t>Acmo</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>APMS-T2</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>APMS-T4</t>
   </si>
   <si>
@@ -113,9 +104,6 @@
     <t>APMS-T6</t>
   </si>
   <si>
-    <t>Vandana C</t>
-  </si>
-  <si>
     <t>APMS-T8</t>
   </si>
   <si>
@@ -158,9 +146,6 @@
     <t>\\TestData\\Excel_Files\\New_Poject_Details.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">Client Image Path </t>
-  </si>
-  <si>
     <t>APMS-T12</t>
   </si>
   <si>
@@ -177,6 +162,42 @@
   </si>
   <si>
     <t>Prashant$123</t>
+  </si>
+  <si>
+    <t>Short project name</t>
+  </si>
+  <si>
+    <t>Automation Dummy project</t>
+  </si>
+  <si>
+    <t>Department name</t>
+  </si>
+  <si>
+    <t>Main contractor name</t>
+  </si>
+  <si>
+    <t>avk</t>
+  </si>
+  <si>
+    <t>Project Type</t>
+  </si>
+  <si>
+    <t>Irrigation</t>
+  </si>
+  <si>
+    <t>Department Image Path</t>
+  </si>
+  <si>
+    <t>Main contractor Image path</t>
+  </si>
+  <si>
+    <t>\\TestData\\Images\\Main_Contractor_logo.png</t>
+  </si>
+  <si>
+    <t>\\TestData\\Images\\Department_Logo.png</t>
+  </si>
+  <si>
+    <t>ATP</t>
   </si>
 </sst>
 </file>
@@ -186,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +222,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="6"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -224,10 +252,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -563,229 +592,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D5353A-A70B-4FBF-B8E0-5139DE62F6E4}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="49.1796875" customWidth="1"/>
-    <col min="6" max="6" width="71.54296875" customWidth="1"/>
-    <col min="8" max="8" width="111.7265625" customWidth="1"/>
+    <col min="3" max="3" width="32.6328125" customWidth="1"/>
+    <col min="8" max="8" width="49.1796875" customWidth="1"/>
+    <col min="9" max="9" width="71.54296875" customWidth="1"/>
+    <col min="11" max="11" width="111.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3">
+        <v>12345678</v>
+      </c>
+      <c r="M3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3">
+        <v>1234567890</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>45418</v>
+      </c>
+      <c r="R3" s="2">
+        <v>45435</v>
+      </c>
+      <c r="S3" s="2">
+        <v>45670</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="K11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3">
-        <v>12345678</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3">
-        <v>1234567890</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="2">
-        <v>45418</v>
-      </c>
-      <c r="O3" s="2">
-        <v>45435</v>
-      </c>
-      <c r="P3" s="2">
-        <v>45670</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" display="prashant@" xr:uid="{420182E3-E264-48AD-9427-74F394420E85}"/>
-    <hyperlink ref="M3" r:id="rId2" xr:uid="{D7A11380-66F9-4EB0-A962-6BBC0383AD52}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{BB4F4B60-A955-431D-9A6F-D674A0235F5F}"/>
-    <hyperlink ref="H3" r:id="rId4" xr:uid="{A5E02953-A716-4FB1-9F94-CBF7B8EB86FB}"/>
-    <hyperlink ref="M8" r:id="rId5" xr:uid="{E466AA4E-62F4-4A07-9470-12321033BF1D}"/>
-    <hyperlink ref="E13" r:id="rId6" xr:uid="{EE9855ED-A36D-4831-BB93-633FEAE35580}"/>
-    <hyperlink ref="E11" r:id="rId7" xr:uid="{118E441C-31E2-4E4A-BAA0-CED89A1941F6}"/>
-    <hyperlink ref="F10" r:id="rId8" xr:uid="{D703EAD6-6487-4B77-90FB-D9AEFE4C648D}"/>
-    <hyperlink ref="H11" r:id="rId9" xr:uid="{9728ACAC-6626-45D1-87FE-2B37E8A86378}"/>
+    <hyperlink ref="N3" r:id="rId1" display="prashant@" xr:uid="{420182E3-E264-48AD-9427-74F394420E85}"/>
+    <hyperlink ref="P3" r:id="rId2" xr:uid="{D7A11380-66F9-4EB0-A962-6BBC0383AD52}"/>
+    <hyperlink ref="I3" r:id="rId3" xr:uid="{BB4F4B60-A955-431D-9A6F-D674A0235F5F}"/>
+    <hyperlink ref="K3" r:id="rId4" xr:uid="{A5E02953-A716-4FB1-9F94-CBF7B8EB86FB}"/>
+    <hyperlink ref="P8" r:id="rId5" xr:uid="{E466AA4E-62F4-4A07-9470-12321033BF1D}"/>
+    <hyperlink ref="H13" r:id="rId6" xr:uid="{EE9855ED-A36D-4831-BB93-633FEAE35580}"/>
+    <hyperlink ref="H11" r:id="rId7" xr:uid="{118E441C-31E2-4E4A-BAA0-CED89A1941F6}"/>
+    <hyperlink ref="I10" r:id="rId8" xr:uid="{D703EAD6-6487-4B77-90FB-D9AEFE4C648D}"/>
+    <hyperlink ref="K11" r:id="rId9" xr:uid="{9728ACAC-6626-45D1-87FE-2B37E8A86378}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>